<commit_message>
vorthanak borrow a book
</commit_message>
<xml_diff>
--- a/borrow.xlsx
+++ b/borrow.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="50">
   <si>
     <t>Book ID [int PK]</t>
   </si>
@@ -171,6 +171,12 @@
   </si>
   <si>
     <t>Black Hat Python</t>
+  </si>
+  <si>
+    <t>The Magic of thinking BIG</t>
+  </si>
+  <si>
+    <t>Hean Vorthanak</t>
   </si>
 </sst>
 </file>
@@ -719,10 +725,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA12"/>
+  <dimension ref="A1:AA13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,6 +1276,41 @@
       </c>
       <c r="O12" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>2016</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13">
+        <v>8</v>
+      </c>
+      <c r="L13">
+        <v>7</v>
+      </c>
+      <c r="M13">
+        <v>2016</v>
+      </c>
+      <c r="O13" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding new content 7/4/2016
</commit_message>
<xml_diff>
--- a/borrow.xlsx
+++ b/borrow.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7530" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="55">
   <si>
     <t>Book ID [int PK]</t>
   </si>
@@ -177,6 +177,21 @@
   </si>
   <si>
     <t>Hean Vorthanak</t>
+  </si>
+  <si>
+    <t>Unity</t>
+  </si>
+  <si>
+    <t>Mai Mom</t>
+  </si>
+  <si>
+    <t>Chay Liheng</t>
+  </si>
+  <si>
+    <t>Android For programmers An app-driven Approach</t>
+  </si>
+  <si>
+    <t>EarlyPhant</t>
   </si>
 </sst>
 </file>
@@ -286,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -310,7 +325,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -322,6 +336,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,10 +701,10 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16"/>
+      <c r="D1" s="15"/>
       <c r="E1" t="s">
         <v>3</v>
       </c>
@@ -725,10 +749,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA13"/>
+  <dimension ref="A1:AA17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="M1" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="I14" sqref="I14:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,11 +773,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
       <c r="D1" s="3" t="s">
         <v>36</v>
       </c>
@@ -764,23 +790,23 @@
       <c r="G1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17" t="s">
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
       <c r="N1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="O1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="17"/>
+      <c r="P1" s="16"/>
       <c r="Q1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1129,73 +1155,91 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:27" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
         <v>22</v>
       </c>
-      <c r="B9">
-        <v>6</v>
-      </c>
-      <c r="C9">
-        <v>2016</v>
-      </c>
-      <c r="D9">
+      <c r="B9" s="12">
+        <v>6</v>
+      </c>
+      <c r="C9" s="12">
+        <v>2016</v>
+      </c>
+      <c r="D9" s="12">
         <v>7</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="K9">
+      <c r="H9" s="12">
+        <v>2</v>
+      </c>
+      <c r="I9" s="12">
+        <v>7</v>
+      </c>
+      <c r="J9" s="12">
+        <v>2016</v>
+      </c>
+      <c r="K9" s="12">
         <v>29</v>
       </c>
-      <c r="L9">
-        <v>6</v>
-      </c>
-      <c r="M9">
-        <v>2016</v>
-      </c>
-      <c r="O9" s="13" t="s">
+      <c r="L9" s="12">
+        <v>6</v>
+      </c>
+      <c r="M9" s="12">
+        <v>2016</v>
+      </c>
+      <c r="O9" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:27" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
         <v>27</v>
       </c>
-      <c r="B10">
-        <v>6</v>
-      </c>
-      <c r="C10">
-        <v>2016</v>
-      </c>
-      <c r="D10">
+      <c r="B10" s="11">
+        <v>6</v>
+      </c>
+      <c r="C10" s="11">
+        <v>2016</v>
+      </c>
+      <c r="D10" s="11">
         <v>8</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="K10">
+      <c r="H10" s="11">
         <v>4</v>
       </c>
-      <c r="L10">
+      <c r="I10" s="11">
         <v>7</v>
       </c>
-      <c r="M10">
-        <v>2016</v>
-      </c>
-      <c r="O10" t="s">
+      <c r="J10" s="11">
+        <v>2016</v>
+      </c>
+      <c r="K10" s="11">
+        <v>4</v>
+      </c>
+      <c r="L10" s="11">
+        <v>7</v>
+      </c>
+      <c r="M10" s="11">
+        <v>2016</v>
+      </c>
+      <c r="O10" s="11" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1313,12 +1357,228 @@
         <v>48</v>
       </c>
     </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" s="19">
+        <v>4</v>
+      </c>
+      <c r="B14" s="19">
+        <v>7</v>
+      </c>
+      <c r="C14" s="19">
+        <v>2016</v>
+      </c>
+      <c r="D14" s="19">
+        <v>12</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="18">
+        <v>11</v>
+      </c>
+      <c r="L14" s="18">
+        <v>7</v>
+      </c>
+      <c r="M14" s="18">
+        <v>2016</v>
+      </c>
+      <c r="N14" s="15"/>
+      <c r="O14" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15"/>
+      <c r="V14" s="15"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="15"/>
+      <c r="Y14" s="15"/>
+      <c r="Z14" s="15"/>
+      <c r="AA14" s="15"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="20"/>
+      <c r="F15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="20"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="15"/>
+      <c r="V15" s="15"/>
+      <c r="W15" s="15"/>
+      <c r="X15" s="15"/>
+      <c r="Y15" s="15"/>
+      <c r="Z15" s="15"/>
+      <c r="AA15" s="15"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16" s="18">
+        <v>4</v>
+      </c>
+      <c r="B16" s="18">
+        <v>7</v>
+      </c>
+      <c r="C16" s="18">
+        <v>2016</v>
+      </c>
+      <c r="D16" s="18">
+        <v>13</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="18">
+        <v>11</v>
+      </c>
+      <c r="L16" s="18">
+        <v>7</v>
+      </c>
+      <c r="M16" s="18">
+        <v>2016</v>
+      </c>
+      <c r="N16" s="15"/>
+      <c r="O16" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="15"/>
+      <c r="W16" s="15"/>
+      <c r="X16" s="15"/>
+      <c r="Y16" s="15"/>
+      <c r="Z16" s="15"/>
+      <c r="AA16" s="15"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="20"/>
+      <c r="F17" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="20"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="15"/>
+      <c r="W17" s="15"/>
+      <c r="X17" s="15"/>
+      <c r="Y17" s="15"/>
+      <c r="Z17" s="15"/>
+      <c r="AA17" s="15"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="56">
+    <mergeCell ref="AA14:AA15"/>
+    <mergeCell ref="AA16:AA17"/>
+    <mergeCell ref="X14:X15"/>
+    <mergeCell ref="X16:X17"/>
+    <mergeCell ref="Y14:Y15"/>
+    <mergeCell ref="Y16:Y17"/>
+    <mergeCell ref="Z14:Z15"/>
+    <mergeCell ref="Z16:Z17"/>
+    <mergeCell ref="U16:U17"/>
+    <mergeCell ref="U14:U15"/>
+    <mergeCell ref="V14:V15"/>
+    <mergeCell ref="V16:V17"/>
+    <mergeCell ref="W16:W17"/>
+    <mergeCell ref="W14:W15"/>
+    <mergeCell ref="S16:S17"/>
+    <mergeCell ref="R14:R15"/>
+    <mergeCell ref="S14:S15"/>
+    <mergeCell ref="T14:T15"/>
+    <mergeCell ref="T16:T17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="Q16:Q17"/>
+    <mergeCell ref="R16:R17"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="O14:O15"/>
+    <mergeCell ref="P14:P15"/>
+    <mergeCell ref="Q14:Q15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="M16:M17"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1326,10 +1586,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,11 +1611,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
       <c r="D1" s="3" t="s">
         <v>36</v>
       </c>
@@ -1368,10 +1628,10 @@
       <c r="G1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="17"/>
+      <c r="I1" s="16"/>
       <c r="J1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1619,6 +1879,58 @@
         <v>46</v>
       </c>
     </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>2016</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>2016</v>
+      </c>
+      <c r="D11">
+        <v>9</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
@@ -1630,10 +1942,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1645,7 +1957,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>43</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -1654,7 +1966,7 @@
       <c r="C1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1703,6 +2015,20 @@
         <v>33</v>
       </c>
       <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="21">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new burrower and return
</commit_message>
<xml_diff>
--- a/borrow.xlsx
+++ b/borrow.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7530" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="57">
   <si>
     <t>Book ID [int PK]</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>EarlyPhant</t>
+  </si>
+  <si>
+    <t>Ro Vinei</t>
+  </si>
+  <si>
+    <t>Hacking - Basic security, Penetration Testing and How to Hack</t>
   </si>
 </sst>
 </file>
@@ -327,6 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -337,15 +344,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,10 +707,10 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15"/>
+      <c r="D1" s="16"/>
       <c r="E1" t="s">
         <v>3</v>
       </c>
@@ -749,12 +755,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA17"/>
+  <dimension ref="A1:AA19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="I14" sqref="I14:I15"/>
+      <selection pane="bottomLeft" activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,11 +779,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
       <c r="D1" s="3" t="s">
         <v>36</v>
       </c>
@@ -790,23 +796,23 @@
       <c r="G1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16" t="s">
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
       <c r="N1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="O1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="16"/>
+      <c r="P1" s="17"/>
       <c r="Q1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1287,38 +1293,47 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:27" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
         <v>29</v>
       </c>
-      <c r="B12">
-        <v>6</v>
-      </c>
-      <c r="C12">
-        <v>2016</v>
-      </c>
-      <c r="D12">
+      <c r="B12" s="12">
+        <v>6</v>
+      </c>
+      <c r="C12" s="12">
+        <v>2016</v>
+      </c>
+      <c r="D12" s="12">
         <v>10</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="K12">
-        <v>6</v>
-      </c>
-      <c r="L12">
-        <v>7</v>
-      </c>
-      <c r="M12">
-        <v>2016</v>
-      </c>
-      <c r="O12" t="s">
+      <c r="H12" s="12">
+        <v>7</v>
+      </c>
+      <c r="I12" s="12">
+        <v>7</v>
+      </c>
+      <c r="J12" s="12">
+        <v>2016</v>
+      </c>
+      <c r="K12" s="12">
+        <v>6</v>
+      </c>
+      <c r="L12" s="12">
+        <v>7</v>
+      </c>
+      <c r="M12" s="12">
+        <v>2016</v>
+      </c>
+      <c r="O12" s="12" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1358,168 +1373,208 @@
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" s="19">
+      <c r="A14" s="20">
         <v>4</v>
       </c>
-      <c r="B14" s="19">
-        <v>7</v>
-      </c>
-      <c r="C14" s="19">
-        <v>2016</v>
-      </c>
-      <c r="D14" s="19">
+      <c r="B14" s="20">
+        <v>7</v>
+      </c>
+      <c r="C14" s="20">
+        <v>2016</v>
+      </c>
+      <c r="D14" s="20">
         <v>12</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="19" t="s">
         <v>50</v>
       </c>
       <c r="F14" t="s">
         <v>51</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="18">
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="21">
         <v>11</v>
       </c>
-      <c r="L14" s="18">
-        <v>7</v>
-      </c>
-      <c r="M14" s="18">
-        <v>2016</v>
-      </c>
-      <c r="N14" s="15"/>
-      <c r="O14" s="20" t="s">
+      <c r="L14" s="21">
+        <v>7</v>
+      </c>
+      <c r="M14" s="21">
+        <v>2016</v>
+      </c>
+      <c r="N14" s="16"/>
+      <c r="O14" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="15"/>
-      <c r="Y14" s="15"/>
-      <c r="Z14" s="15"/>
-      <c r="AA14" s="15"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="16"/>
+      <c r="U14" s="16"/>
+      <c r="V14" s="16"/>
+      <c r="W14" s="16"/>
+      <c r="X14" s="16"/>
+      <c r="Y14" s="16"/>
+      <c r="Z14" s="16"/>
+      <c r="AA14" s="16"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="20"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="19"/>
       <c r="F15" t="s">
         <v>52</v>
       </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="15"/>
-      <c r="U15" s="15"/>
-      <c r="V15" s="15"/>
-      <c r="W15" s="15"/>
-      <c r="X15" s="15"/>
-      <c r="Y15" s="15"/>
-      <c r="Z15" s="15"/>
-      <c r="AA15" s="15"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="16"/>
+      <c r="U15" s="16"/>
+      <c r="V15" s="16"/>
+      <c r="W15" s="16"/>
+      <c r="X15" s="16"/>
+      <c r="Y15" s="16"/>
+      <c r="Z15" s="16"/>
+      <c r="AA15" s="16"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="18">
+      <c r="A16" s="21">
         <v>4</v>
       </c>
-      <c r="B16" s="18">
-        <v>7</v>
-      </c>
-      <c r="C16" s="18">
-        <v>2016</v>
-      </c>
-      <c r="D16" s="18">
+      <c r="B16" s="21">
+        <v>7</v>
+      </c>
+      <c r="C16" s="21">
+        <v>2016</v>
+      </c>
+      <c r="D16" s="21">
         <v>13</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="19" t="s">
         <v>54</v>
       </c>
       <c r="F16" t="s">
         <v>38</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="G16" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="18">
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="21">
         <v>11</v>
       </c>
-      <c r="L16" s="18">
-        <v>7</v>
-      </c>
-      <c r="M16" s="18">
-        <v>2016</v>
-      </c>
-      <c r="N16" s="15"/>
-      <c r="O16" s="20" t="s">
+      <c r="L16" s="21">
+        <v>7</v>
+      </c>
+      <c r="M16" s="21">
+        <v>2016</v>
+      </c>
+      <c r="N16" s="16"/>
+      <c r="O16" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15"/>
-      <c r="X16" s="15"/>
-      <c r="Y16" s="15"/>
-      <c r="Z16" s="15"/>
-      <c r="AA16" s="15"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16"/>
+      <c r="U16" s="16"/>
+      <c r="V16" s="16"/>
+      <c r="W16" s="16"/>
+      <c r="X16" s="16"/>
+      <c r="Y16" s="16"/>
+      <c r="Z16" s="16"/>
+      <c r="AA16" s="16"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="20"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="19"/>
       <c r="F17" t="s">
         <v>49</v>
       </c>
-      <c r="G17" s="20"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="20"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="15"/>
-      <c r="T17" s="15"/>
-      <c r="U17" s="15"/>
-      <c r="V17" s="15"/>
-      <c r="W17" s="15"/>
-      <c r="X17" s="15"/>
-      <c r="Y17" s="15"/>
-      <c r="Z17" s="15"/>
-      <c r="AA17" s="15"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="16"/>
+      <c r="V17" s="16"/>
+      <c r="W17" s="16"/>
+      <c r="X17" s="16"/>
+      <c r="Y17" s="16"/>
+      <c r="Z17" s="16"/>
+      <c r="AA17" s="16"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>2016</v>
+      </c>
+      <c r="D19">
+        <v>15</v>
+      </c>
+      <c r="E19" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" t="s">
+        <v>30</v>
+      </c>
+      <c r="K19">
+        <v>15</v>
+      </c>
+      <c r="L19">
+        <v>7</v>
+      </c>
+      <c r="M19">
+        <v>2016</v>
+      </c>
+      <c r="O19" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="56">
@@ -1586,10 +1641,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T11"/>
+  <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1611,11 +1666,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
       <c r="D1" s="3" t="s">
         <v>36</v>
       </c>
@@ -1628,10 +1683,10 @@
       <c r="G1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="16"/>
+      <c r="I1" s="17"/>
       <c r="J1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1931,6 +1986,32 @@
         <v>39</v>
       </c>
     </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>2016</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
@@ -1942,10 +2023,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2028,7 +2109,21 @@
       <c r="C6" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="15">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new burrow and ewnew
</commit_message>
<xml_diff>
--- a/borrow.xlsx
+++ b/borrow.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="borrow" sheetId="2" r:id="rId2"/>
-    <sheet name="Paid" sheetId="3" r:id="rId3"/>
+    <sheet name="Return" sheetId="3" r:id="rId3"/>
     <sheet name="Late borrower" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="60">
   <si>
     <t>Book ID [int PK]</t>
   </si>
@@ -198,6 +198,15 @@
   </si>
   <si>
     <t>Hacking - Basic security, Penetration Testing and How to Hack</t>
+  </si>
+  <si>
+    <t>Loem Kimhak</t>
+  </si>
+  <si>
+    <t>Kimhak Loem</t>
+  </si>
+  <si>
+    <t>Rich Dad, Poor Dad - FBSI</t>
   </si>
 </sst>
 </file>
@@ -307,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -337,6 +346,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -344,13 +359,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -755,12 +773,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA19"/>
+  <dimension ref="A1:AA22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="O12" sqref="O12"/>
+      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,7 +789,7 @@
     <col min="10" max="12" width="9.7109375" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="56.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="23.5703125" customWidth="1"/>
     <col min="17" max="17" width="21.28515625" customWidth="1"/>
     <col min="18" max="19" width="19.28515625" customWidth="1"/>
@@ -779,11 +797,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
       <c r="D1" s="3" t="s">
         <v>36</v>
       </c>
@@ -796,23 +814,23 @@
       <c r="G1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17" t="s">
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
       <c r="N1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="O1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="17"/>
+      <c r="P1" s="19"/>
       <c r="Q1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1373,41 +1391,41 @@
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" s="20">
+      <c r="A14" s="21">
         <v>4</v>
       </c>
-      <c r="B14" s="20">
-        <v>7</v>
-      </c>
-      <c r="C14" s="20">
-        <v>2016</v>
-      </c>
-      <c r="D14" s="20">
+      <c r="B14" s="21">
+        <v>7</v>
+      </c>
+      <c r="C14" s="21">
+        <v>2016</v>
+      </c>
+      <c r="D14" s="21">
         <v>12</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="17" t="s">
         <v>50</v>
       </c>
       <c r="F14" t="s">
         <v>51</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="17" t="s">
         <v>30</v>
       </c>
       <c r="H14" s="16"/>
       <c r="I14" s="16"/>
       <c r="J14" s="16"/>
-      <c r="K14" s="21">
+      <c r="K14" s="18">
         <v>11</v>
       </c>
-      <c r="L14" s="21">
-        <v>7</v>
-      </c>
-      <c r="M14" s="21">
+      <c r="L14" s="18">
+        <v>7</v>
+      </c>
+      <c r="M14" s="18">
         <v>2016</v>
       </c>
       <c r="N14" s="16"/>
-      <c r="O14" s="19" t="s">
+      <c r="O14" s="17" t="s">
         <v>53</v>
       </c>
       <c r="P14" s="16"/>
@@ -1424,23 +1442,23 @@
       <c r="AA14" s="16"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="19"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="17"/>
       <c r="F15" t="s">
         <v>52</v>
       </c>
-      <c r="G15" s="19"/>
+      <c r="G15" s="17"/>
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
       <c r="N15" s="16"/>
-      <c r="O15" s="19"/>
+      <c r="O15" s="17"/>
       <c r="P15" s="16"/>
       <c r="Q15" s="16"/>
       <c r="R15" s="16"/>
@@ -1454,87 +1472,87 @@
       <c r="Z15" s="16"/>
       <c r="AA15" s="16"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="21">
+    <row r="16" spans="1:27" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="22">
         <v>4</v>
       </c>
-      <c r="B16" s="21">
-        <v>7</v>
-      </c>
-      <c r="C16" s="21">
-        <v>2016</v>
-      </c>
-      <c r="D16" s="21">
+      <c r="B16" s="22">
+        <v>7</v>
+      </c>
+      <c r="C16" s="22">
+        <v>2016</v>
+      </c>
+      <c r="D16" s="22">
         <v>13</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="G16" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="21">
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="22">
         <v>11</v>
       </c>
-      <c r="L16" s="21">
-        <v>7</v>
-      </c>
-      <c r="M16" s="21">
-        <v>2016</v>
-      </c>
-      <c r="N16" s="16"/>
-      <c r="O16" s="19" t="s">
+      <c r="L16" s="22">
+        <v>7</v>
+      </c>
+      <c r="M16" s="22">
+        <v>2016</v>
+      </c>
+      <c r="N16" s="24"/>
+      <c r="O16" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="16"/>
-      <c r="S16" s="16"/>
-      <c r="T16" s="16"/>
-      <c r="U16" s="16"/>
-      <c r="V16" s="16"/>
-      <c r="W16" s="16"/>
-      <c r="X16" s="16"/>
-      <c r="Y16" s="16"/>
-      <c r="Z16" s="16"/>
-      <c r="AA16" s="16"/>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="19"/>
-      <c r="F17" t="s">
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="24"/>
+      <c r="S16" s="24"/>
+      <c r="T16" s="24"/>
+      <c r="U16" s="24"/>
+      <c r="V16" s="24"/>
+      <c r="W16" s="24"/>
+      <c r="X16" s="24"/>
+      <c r="Y16" s="24"/>
+      <c r="Z16" s="24"/>
+      <c r="AA16" s="24"/>
+    </row>
+    <row r="17" spans="1:27" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="G17" s="19"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="16"/>
-      <c r="O17" s="19"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="16"/>
-      <c r="S17" s="16"/>
-      <c r="T17" s="16"/>
-      <c r="U17" s="16"/>
-      <c r="V17" s="16"/>
-      <c r="W17" s="16"/>
-      <c r="X17" s="16"/>
-      <c r="Y17" s="16"/>
-      <c r="Z17" s="16"/>
-      <c r="AA17" s="16"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="24"/>
+      <c r="S17" s="24"/>
+      <c r="T17" s="24"/>
+      <c r="U17" s="24"/>
+      <c r="V17" s="24"/>
+      <c r="W17" s="24"/>
+      <c r="X17" s="24"/>
+      <c r="Y17" s="24"/>
+      <c r="Z17" s="24"/>
+      <c r="AA17" s="24"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="D18">
@@ -1576,32 +1594,131 @@
         <v>56</v>
       </c>
     </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>11</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>2016</v>
+      </c>
+      <c r="D20">
+        <v>16</v>
+      </c>
+      <c r="E20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" t="s">
+        <v>30</v>
+      </c>
+      <c r="K20">
+        <v>18</v>
+      </c>
+      <c r="L20">
+        <v>7</v>
+      </c>
+      <c r="M20">
+        <v>2016</v>
+      </c>
+      <c r="O20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A21" s="18">
+        <v>11</v>
+      </c>
+      <c r="B21" s="18">
+        <v>7</v>
+      </c>
+      <c r="C21" s="18">
+        <v>2016</v>
+      </c>
+      <c r="D21" s="18">
+        <v>17</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="18">
+        <v>18</v>
+      </c>
+      <c r="L21" s="18">
+        <v>7</v>
+      </c>
+      <c r="M21" s="18">
+        <v>2016</v>
+      </c>
+      <c r="N21" s="16"/>
+      <c r="O21" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="17"/>
+      <c r="F22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" s="17"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="17"/>
+    </row>
   </sheetData>
-  <mergeCells count="56">
-    <mergeCell ref="AA14:AA15"/>
-    <mergeCell ref="AA16:AA17"/>
-    <mergeCell ref="X14:X15"/>
-    <mergeCell ref="X16:X17"/>
-    <mergeCell ref="Y14:Y15"/>
-    <mergeCell ref="Y16:Y17"/>
-    <mergeCell ref="Z14:Z15"/>
-    <mergeCell ref="Z16:Z17"/>
-    <mergeCell ref="U16:U17"/>
-    <mergeCell ref="U14:U15"/>
-    <mergeCell ref="V14:V15"/>
-    <mergeCell ref="V16:V17"/>
-    <mergeCell ref="W16:W17"/>
-    <mergeCell ref="W14:W15"/>
-    <mergeCell ref="S16:S17"/>
-    <mergeCell ref="R14:R15"/>
-    <mergeCell ref="S14:S15"/>
-    <mergeCell ref="T14:T15"/>
-    <mergeCell ref="T16:T17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="P16:P17"/>
-    <mergeCell ref="Q16:Q17"/>
-    <mergeCell ref="R16:R17"/>
+  <mergeCells count="70">
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="O21:O22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
     <mergeCell ref="N14:N15"/>
     <mergeCell ref="O14:O15"/>
     <mergeCell ref="P14:P15"/>
@@ -1618,22 +1735,30 @@
     <mergeCell ref="K16:K17"/>
     <mergeCell ref="L16:L17"/>
     <mergeCell ref="M16:M17"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="Q16:Q17"/>
+    <mergeCell ref="R16:R17"/>
+    <mergeCell ref="S16:S17"/>
+    <mergeCell ref="R14:R15"/>
+    <mergeCell ref="S14:S15"/>
+    <mergeCell ref="T14:T15"/>
+    <mergeCell ref="T16:T17"/>
+    <mergeCell ref="U16:U17"/>
+    <mergeCell ref="U14:U15"/>
+    <mergeCell ref="V14:V15"/>
+    <mergeCell ref="V16:V17"/>
+    <mergeCell ref="W16:W17"/>
+    <mergeCell ref="W14:W15"/>
+    <mergeCell ref="AA14:AA15"/>
+    <mergeCell ref="AA16:AA17"/>
+    <mergeCell ref="X14:X15"/>
+    <mergeCell ref="X16:X17"/>
+    <mergeCell ref="Y14:Y15"/>
+    <mergeCell ref="Y16:Y17"/>
+    <mergeCell ref="Z14:Z15"/>
+    <mergeCell ref="Z16:Z17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1641,10 +1766,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:F12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1666,11 +1791,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
       <c r="D1" s="3" t="s">
         <v>36</v>
       </c>
@@ -1683,10 +1808,10 @@
       <c r="G1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="17"/>
+      <c r="I1" s="19"/>
       <c r="J1" s="3" t="s">
         <v>3</v>
       </c>
@@ -2012,6 +2137,32 @@
         <v>47</v>
       </c>
     </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>2016</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
@@ -2026,7 +2177,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>